<commit_message>
updated status of theses
</commit_message>
<xml_diff>
--- a/Abschlussarbeiten.xlsx
+++ b/Abschlussarbeiten.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t>Name der Arbeit</t>
   </si>
@@ -76,14 +76,6 @@
     <t>Zeynep Günes</t>
   </si>
   <si>
-    <t>Aufbau eines
-Sprachkorpus zur
-Programmierung
-autonomer Roboter
-mittels natürlicher
-Sprache</t>
-  </si>
-  <si>
     <t>Dinesh Paskaran</t>
   </si>
   <si>
@@ -100,6 +92,22 @@
   </si>
   <si>
     <t>09.01.15 - 08.05.15</t>
+  </si>
+  <si>
+    <t>01.04.15. - 31.07.15</t>
+  </si>
+  <si>
+    <t>Ja, bis 22.05.15</t>
+  </si>
+  <si>
+    <t>Projektion von gesprochener Sprache auf eine Handlungsrepräsentation</t>
+  </si>
+  <si>
+    <t>Aufbau eines Sprachkorpus zur Programmierung autonomer Roboter
+mittels natürlicher Sprache</t>
+  </si>
+  <si>
+    <t>Entwurf einer Handlungsrepräsentation für gesprochene Sprache (ehem. 'Entwurf einer logischen Repräsentation für gesprochene Sprache')</t>
   </si>
 </sst>
 </file>
@@ -164,12 +172,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -193,13 +197,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -216,6 +235,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -236,6 +256,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border outline="0">
         <right style="thin">
           <color rgb="FF3F3F3F"/>
@@ -256,20 +277,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L18" totalsRowShown="0" headerRowCellStyle="Output" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:L18" totalsRowShown="0" dataDxfId="0" headerRowCellStyle="Output" dataCellStyle="Output">
   <autoFilter ref="B2:L18"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Name der Arbeit" dataDxfId="10" dataCellStyle="Output"/>
-    <tableColumn id="2" name="Typ" dataDxfId="9" dataCellStyle="Output"/>
-    <tableColumn id="3" name="Bearbeiter" dataDxfId="8" dataCellStyle="Output"/>
-    <tableColumn id="4" name="Exposé-Status" dataDxfId="7" dataCellStyle="Output"/>
-    <tableColumn id="5" name="Angemeldet" dataDxfId="6" dataCellStyle="Output"/>
-    <tableColumn id="6" name="Bearbeitungszeitraum" dataDxfId="5" dataCellStyle="Output"/>
-    <tableColumn id="7" name="Abgegeben" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="9" name="Verlängert" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="10" name="Termin Vortrag" dataDxfId="2" dataCellStyle="Output"/>
-    <tableColumn id="8" name="Note" dataDxfId="1" dataCellStyle="Output"/>
-    <tableColumn id="11" name="Anmerkungen" dataDxfId="0" dataCellStyle="Output"/>
+    <tableColumn id="1" name="Name der Arbeit" dataDxfId="11" dataCellStyle="Output"/>
+    <tableColumn id="2" name="Typ" dataDxfId="10" dataCellStyle="Output"/>
+    <tableColumn id="3" name="Bearbeiter" dataDxfId="9" dataCellStyle="Output"/>
+    <tableColumn id="4" name="Exposé-Status" dataDxfId="8" dataCellStyle="Output"/>
+    <tableColumn id="5" name="Angemeldet" dataDxfId="7" dataCellStyle="Output"/>
+    <tableColumn id="6" name="Bearbeitungszeitraum" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="7" name="Abgegeben" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="9" name="Verlängert" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="10" name="Termin Vortrag" dataDxfId="3" dataCellStyle="Output"/>
+    <tableColumn id="8" name="Note" dataDxfId="2" dataCellStyle="Output"/>
+    <tableColumn id="11" name="Anmerkungen" dataDxfId="1" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -565,332 +586,348 @@
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="17" style="7" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="7"/>
-    <col min="12" max="12" width="45.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="17" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="45.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="9">
+        <v>42167</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="9">
+        <v>42167</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>22</v>
+      <c r="L4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="5"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="5"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="5"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="5"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="5"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="5"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="5"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="5"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="5"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>